<commit_message>
major refactor to typescript, added 2023 records
</commit_message>
<xml_diff>
--- a/data/team_names.xlsx
+++ b/data/team_names.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msimoni/repos/mo-chicken.git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4105BF7-D309-9A47-822C-08938E5FF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612B0390-D5D5-1E48-BD08-8734D6603525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31860" yWindow="2080" windowWidth="12140" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="760" windowWidth="28360" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Names" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Names!$A$1:$C$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Names!$A$1:$C$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="63">
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
   <si>
     <t>Shmo Stars</t>
   </si>
@@ -160,9 +158,6 @@
     <t>Route 28 Speed Walkers</t>
   </si>
   <si>
-    <t>Manager</t>
-  </si>
-  <si>
     <t>Moni</t>
   </si>
   <si>
@@ -220,10 +215,37 @@
     <t>Burgs downfall</t>
   </si>
   <si>
-    <t>Waiver Wire Weiners</t>
-  </si>
-  <si>
     <t>Out of Timers</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Waiver Wire Wieners</t>
+  </si>
+  <si>
+    <t>Wieners UpRising</t>
+  </si>
+  <si>
+    <t>Mollywhoppers</t>
+  </si>
+  <si>
+    <t>Auto draft</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Count of year</t>
   </si>
 </sst>
 </file>
@@ -286,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -294,6 +316,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -310,6 +337,470 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45512.9350150463" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="76" xr:uid="{F0829A66-9B71-744C-84CF-A3DA58709B23}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:C77" sheet="Names"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="manager" numFmtId="0">
+      <sharedItems count="15">
+        <s v="?"/>
+        <s v="AK"/>
+        <s v="Burg"/>
+        <s v="Ciggy"/>
+        <s v="Dane"/>
+        <s v="Het"/>
+        <s v="Jake"/>
+        <s v="Kyle"/>
+        <s v="Marsh"/>
+        <s v="Masi"/>
+        <s v="Moni"/>
+        <s v="Phil"/>
+        <s v="Shoey"/>
+        <s v="Stew"/>
+        <s v="Zach"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2014" maxValue="2021" count="8">
+        <n v="2015"/>
+        <n v="2014"/>
+        <n v="2016"/>
+        <n v="2017"/>
+        <n v="2018"/>
+        <n v="2019"/>
+        <n v="2020"/>
+        <n v="2021"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="76">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECB7068A-9217-E545-BBBB-20DB1AEF4F30}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="9">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of year" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,11 +1087,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C4BD63-91D5-934C-A12D-D0B87023F154}">
+  <dimension ref="A3:B19"/>
+  <sheetViews>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="4">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V93"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -611,13 +1259,13 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -639,10 +1287,10 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>2015</v>
@@ -650,10 +1298,10 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -661,10 +1309,10 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>2015</v>
@@ -672,10 +1320,10 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>2016</v>
@@ -683,10 +1331,10 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>2017</v>
@@ -694,10 +1342,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>2018</v>
@@ -705,10 +1353,10 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>2019</v>
@@ -716,10 +1364,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>2020</v>
@@ -727,10 +1375,10 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>2021</v>
@@ -738,406 +1386,406 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11">
-        <v>2014</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12">
-        <v>2015</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>2014</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20">
-        <v>2015</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C21">
-        <v>2016</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22">
-        <v>2017</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C23">
-        <v>2018</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24">
-        <v>2019</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26">
-        <v>2021</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C27">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C28">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C29">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C30">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C31">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C32">
-        <v>2018</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>51</v>
       </c>
       <c r="C34">
-        <v>2020</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
         <v>51</v>
       </c>
       <c r="C35">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36">
-        <v>2014</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C38">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C40">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C41">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C43">
-        <v>2018</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C44">
-        <v>2019</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46">
-        <v>2021</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C47">
         <v>2014</v>
@@ -1145,10 +1793,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C48">
         <v>2015</v>
@@ -1156,10 +1804,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C49">
         <v>2016</v>
@@ -1167,10 +1815,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C50">
         <v>2017</v>
@@ -1178,10 +1826,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C51">
         <v>2018</v>
@@ -1189,10 +1837,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C52">
         <v>2019</v>
@@ -1200,10 +1848,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C53">
         <v>2020</v>
@@ -1211,10 +1859,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C54">
         <v>2021</v>
@@ -1222,249 +1870,249 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C55">
-        <v>2014</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C56">
-        <v>2015</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C57">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C58">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C59">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C60">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C61">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C62">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C63">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C64">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C65">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C66">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C67">
-        <v>2021</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C68">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C69">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C70">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C71">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C72">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C73">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C74">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C75">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C76">
-        <v>2014</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
         <v>50</v>
@@ -1475,68 +2123,68 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C78">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C79">
-        <v>2017</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B80" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C80">
-        <v>2018</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B81" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C81">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B82" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C82">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C83">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1544,95 +2192,95 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C84">
-        <v>2022</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
         <v>45</v>
       </c>
       <c r="C85">
-        <v>2022</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C86">
-        <v>2022</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C87">
-        <v>2022</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C88">
-        <v>2022</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C89">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C90">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C91">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C92">
         <v>2022</v>
@@ -1640,19 +2288,129 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B93" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C93">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>47</v>
+      </c>
+      <c r="C95">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>47</v>
+      </c>
+      <c r="C96">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>47</v>
+      </c>
+      <c r="C101">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C102">
         <v>2022</v>
       </c>
     </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>47</v>
+      </c>
+      <c r="C103">
+        <v>2023</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C83">
-    <sortCondition ref="B2:B83"/>
-    <sortCondition ref="C2:C83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C103">
+    <sortCondition ref="B2:B103"/>
+    <sortCondition ref="C2:C103"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated site for 2024 season
</commit_message>
<xml_diff>
--- a/data/team_names.xlsx
+++ b/data/team_names.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msimoni/repos/mo-chicken.git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612B0390-D5D5-1E48-BD08-8734D6603525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BD0782-C2CF-8F49-B493-10A3B5F7F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="760" windowWidth="28360" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="760" windowWidth="27800" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Names" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Names!$A$1:$C$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Names!$A$1:$C$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="70">
   <si>
     <t>Shmo Stars</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Count of year</t>
+  </si>
+  <si>
+    <t>Sergeant Friendly</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -317,7 +320,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -695,7 +697,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECB7068A-9217-E545-BBBB-20DB1AEF4F30}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECB7068A-9217-E545-BBBB-20DB1AEF4F30}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -1103,7 +1105,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" t="s">
@@ -1111,130 +1113,130 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>76</v>
       </c>
     </row>
@@ -1245,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V103"/>
+  <dimension ref="A1:V113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1287,21 +1289,21 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
       </c>
       <c r="C2">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -1309,112 +1311,112 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C5">
-        <v>2016</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C6">
-        <v>2017</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>2018</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8">
-        <v>2019</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10">
-        <v>2021</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11">
-        <v>2022</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C12">
-        <v>2023</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -1430,120 +1432,120 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C16">
-        <v>2017</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C17">
-        <v>2018</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C18">
-        <v>2019</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C19">
-        <v>2020</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20">
-        <v>2021</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>2022</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C22">
-        <v>2023</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C23">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25">
         <v>2016</v>
@@ -1551,87 +1553,87 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
       <c r="C26">
-        <v>2017</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C27">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C30">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31">
-        <v>2022</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C32">
-        <v>2023</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C33">
         <v>2016</v>
@@ -1639,35 +1641,35 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C34">
-        <v>2014</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C36">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1683,112 +1685,112 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C38">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C39">
-        <v>2019</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40">
-        <v>2020</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>2021</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>2022</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43">
-        <v>2023</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C44">
-        <v>2014</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C45">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C46">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C47">
-        <v>2014</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1799,37 +1801,37 @@
         <v>44</v>
       </c>
       <c r="C48">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C49">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C50">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C51">
         <v>2018</v>
@@ -1837,79 +1839,79 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C52">
-        <v>2019</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C54">
-        <v>2021</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C55">
-        <v>2022</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C56">
-        <v>2023</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C57">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C58">
-        <v>2015</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1920,37 +1922,37 @@
         <v>46</v>
       </c>
       <c r="C59">
-        <v>2016</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C60">
-        <v>2017</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C61">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C62">
         <v>2019</v>
@@ -1958,120 +1960,120 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C63">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C64">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C65">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C66">
-        <v>2023</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C67">
-        <v>2014</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C68">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C69">
-        <v>2016</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B70" t="s">
         <v>39</v>
       </c>
       <c r="C70">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C71">
-        <v>2018</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C72">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C73">
         <v>2020</v>
@@ -2079,10 +2081,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C74">
         <v>2021</v>
@@ -2090,68 +2092,68 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C75">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C76">
-        <v>2023</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C77">
-        <v>2015</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B78" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C78">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C79">
-        <v>2019</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C80">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2167,112 +2169,112 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C82">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C83">
-        <v>2023</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B84" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C84">
-        <v>2014</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B85" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C85">
-        <v>2015</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B86" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C86">
-        <v>2016</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B87" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C87">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C88">
-        <v>2018</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C89">
-        <v>2019</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B90" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C90">
-        <v>2020</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="B91" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C91">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2288,112 +2290,112 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B93" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C93">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="B94" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C94">
-        <v>2014</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B95" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C95">
-        <v>2015</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="B96" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C96">
-        <v>2016</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C97">
-        <v>2017</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B98" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C98">
-        <v>2018</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C99">
-        <v>2019</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B100" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C100">
-        <v>2020</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B101" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C101">
-        <v>2021</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C102">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,6 +2407,116 @@
       </c>
       <c r="C103">
         <v>2023</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>63</v>
+      </c>
+      <c r="B104" t="s">
+        <v>43</v>
+      </c>
+      <c r="C104">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>56</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>33</v>
+      </c>
+      <c r="B107" t="s">
+        <v>48</v>
+      </c>
+      <c r="C107">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" t="s">
+        <v>44</v>
+      </c>
+      <c r="C108">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>69</v>
+      </c>
+      <c r="B109" t="s">
+        <v>46</v>
+      </c>
+      <c r="C109">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>65</v>
+      </c>
+      <c r="B111" t="s">
+        <v>42</v>
+      </c>
+      <c r="C111">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>64</v>
+      </c>
+      <c r="B112" t="s">
+        <v>45</v>
+      </c>
+      <c r="C112">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>47</v>
+      </c>
+      <c r="C113">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>